<commit_message>
Allow full switch to bio options in IND by 2050
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_IND_Mitigations.xlsx
+++ b/SuppXLS/Scen_IND_Mitigations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\TIMES-Ireland-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D715A1-BDC3-4E1C-8E50-E387F68FA1BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F29C1-0014-491A-AE21-984D6082B117}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -2001,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE22" sqref="AE22"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W81" sqref="W81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="O12" s="37">
         <f>O7*T12</f>
-        <v>3.4999999999999996E-3</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="P12">
         <v>5</v>
@@ -2665,7 +2665,7 @@
         <v>0.3</v>
       </c>
       <c r="T12" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V12" s="17"/>
       <c r="W12" s="17"/>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="O13" s="37">
         <f t="shared" si="2"/>
-        <v>0.20849000000000001</v>
+        <v>0.41698000000000002</v>
       </c>
       <c r="P13">
         <v>5</v>
@@ -2755,7 +2755,7 @@
         <v>0.3</v>
       </c>
       <c r="T13" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V13" t="s">
         <v>130</v>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="O14" s="36">
         <f t="shared" si="2"/>
-        <v>8.8800000000000004E-2</v>
+        <v>0.17760000000000001</v>
       </c>
       <c r="P14" s="16">
         <v>5</v>
@@ -2814,7 +2814,7 @@
         <v>0.3</v>
       </c>
       <c r="T14" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V14" s="16" t="s">
         <v>130</v>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="O24" s="37">
         <f>O22*T24</f>
-        <v>0.249775</v>
+        <v>0.49954999999999999</v>
       </c>
       <c r="P24">
         <v>5</v>
@@ -3471,7 +3471,7 @@
         <v>0.3</v>
       </c>
       <c r="T24" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V24" s="51" t="s">
         <v>130</v>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="O26" s="37">
         <f>O18*T26</f>
-        <v>1.9450000000000001E-3</v>
+        <v>3.8900000000000002E-3</v>
       </c>
       <c r="P26">
         <v>5</v>
@@ -3575,7 +3575,7 @@
         <v>0.3</v>
       </c>
       <c r="T26" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V26" s="51" t="s">
         <v>130</v>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="O27" s="36">
         <f>O21*T27</f>
-        <v>1.5139999999999999E-2</v>
+        <v>3.0279999999999998E-2</v>
       </c>
       <c r="P27" s="16">
         <v>5</v>
@@ -3634,7 +3634,7 @@
         <v>0.3</v>
       </c>
       <c r="T27" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V27" s="51" t="s">
         <v>130</v>
@@ -4123,7 +4123,7 @@
       </c>
       <c r="O34" s="35">
         <f>O29*T34</f>
-        <v>1.08E-3</v>
+        <v>2.16E-3</v>
       </c>
       <c r="P34">
         <v>5</v>
@@ -4135,7 +4135,7 @@
         <v>0.3</v>
       </c>
       <c r="T34" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V34" s="19"/>
       <c r="X34" s="41" t="str">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="O35" s="35">
         <f t="shared" si="7"/>
-        <v>1.2104999999999999E-2</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="P35">
         <v>5</v>
@@ -4221,7 +4221,7 @@
         <v>0.3</v>
       </c>
       <c r="T35" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V35" t="s">
         <v>130</v>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="O36" s="36">
         <f t="shared" si="7"/>
-        <v>0.34546499999999997</v>
+        <v>0.69092999999999993</v>
       </c>
       <c r="P36" s="16">
         <v>5</v>
@@ -4274,7 +4274,7 @@
         <v>0.3</v>
       </c>
       <c r="T36" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V36" t="s">
         <v>130</v>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="O44" s="35">
         <f>O38*T44</f>
-        <v>2.8000000000000003E-4</v>
+        <v>5.6000000000000006E-4</v>
       </c>
       <c r="P44">
         <v>5</v>
@@ -4843,7 +4843,7 @@
         <v>0.3</v>
       </c>
       <c r="T44" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V44" s="19" t="s">
         <v>130</v>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="O45" s="35">
         <f t="shared" si="17"/>
-        <v>7.025E-3</v>
+        <v>1.405E-2</v>
       </c>
       <c r="P45">
         <v>5</v>
@@ -4902,7 +4902,7 @@
         <v>0.3</v>
       </c>
       <c r="T45" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V45" s="19" t="s">
         <v>130</v>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="O46" s="36">
         <f t="shared" si="17"/>
-        <v>9.4599999999999997E-3</v>
+        <v>1.8919999999999999E-2</v>
       </c>
       <c r="P46" s="16">
         <v>5</v>
@@ -4961,7 +4961,7 @@
         <v>0.3</v>
       </c>
       <c r="T46" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V46" s="19" t="s">
         <v>130</v>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="O53" s="35">
         <f>O48*T53</f>
-        <v>6.0699999999999999E-3</v>
+        <v>1.214E-2</v>
       </c>
       <c r="P53">
         <v>5</v>
@@ -5462,7 +5462,7 @@
         <v>0.3</v>
       </c>
       <c r="T53" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X53" s="41" t="str">
         <f>X52</f>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="O54" s="35">
         <f t="shared" si="26"/>
-        <v>1.8435E-2</v>
+        <v>3.687E-2</v>
       </c>
       <c r="P54">
         <v>5</v>
@@ -5547,7 +5547,7 @@
         <v>0.3</v>
       </c>
       <c r="T54" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V54" t="s">
         <v>130</v>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="O55" s="36">
         <f t="shared" si="26"/>
-        <v>0.14293</v>
+        <v>0.28586</v>
       </c>
       <c r="P55" s="16">
         <v>5</v>
@@ -5606,7 +5606,7 @@
         <v>0.3</v>
       </c>
       <c r="T55" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V55" t="s">
         <v>130</v>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="O64" s="35">
         <f>O57*T64</f>
-        <v>5.8E-4</v>
+        <v>1.16E-3</v>
       </c>
       <c r="P64">
         <v>5</v>
@@ -6174,7 +6174,7 @@
         <v>0.3</v>
       </c>
       <c r="T64" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V64" s="19" t="s">
         <v>130</v>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="O65" s="35">
         <f>O60*T65</f>
-        <v>9.6950000000000005E-3</v>
+        <v>1.9390000000000001E-2</v>
       </c>
       <c r="P65">
         <v>5</v>
@@ -6221,7 +6221,7 @@
         <v>0.3</v>
       </c>
       <c r="T65" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V65" s="19" t="s">
         <v>130</v>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="O66" s="36">
         <f>O62*T66</f>
-        <v>0.25284999999999996</v>
+        <v>0.50569999999999993</v>
       </c>
       <c r="P66" s="16">
         <v>5</v>
@@ -6268,7 +6268,7 @@
         <v>0.3</v>
       </c>
       <c r="T66" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V66" s="19" t="s">
         <v>130</v>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="O73" s="35">
         <f>O68*T73</f>
-        <v>3.3764999999999996E-2</v>
+        <v>6.7529999999999993E-2</v>
       </c>
       <c r="P73">
         <v>5</v>
@@ -6697,7 +6697,7 @@
         <v>0.3</v>
       </c>
       <c r="T73" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V73" s="19"/>
       <c r="W73" s="19"/>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="O74" s="35">
         <f t="shared" si="46"/>
-        <v>2.6545000000000003E-2</v>
+        <v>5.3090000000000005E-2</v>
       </c>
       <c r="P74" s="19">
         <v>5</v>
@@ -6772,7 +6772,7 @@
         <v>0.3</v>
       </c>
       <c r="T74" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V74" t="s">
         <v>130</v>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="O75" s="36">
         <f t="shared" si="46"/>
-        <v>4.1924999999999997E-2</v>
+        <v>8.3849999999999994E-2</v>
       </c>
       <c r="P75" s="16">
         <v>5</v>
@@ -6819,7 +6819,7 @@
         <v>0.3</v>
       </c>
       <c r="T75" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V75" t="s">
         <v>130</v>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="O87" s="35">
         <f>O78*T87</f>
-        <v>2.0149999999999999E-3</v>
+        <v>4.0299999999999997E-3</v>
       </c>
       <c r="P87" s="19">
         <v>5</v>
@@ -7432,7 +7432,7 @@
         <v>0.3</v>
       </c>
       <c r="T87" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V87" s="19" t="s">
         <v>130</v>
@@ -7467,7 +7467,7 @@
       </c>
       <c r="O88" s="35">
         <f>O80*T88</f>
-        <v>3.5119999999999998E-2</v>
+        <v>7.0239999999999997E-2</v>
       </c>
       <c r="P88" s="19">
         <v>5</v>
@@ -7479,7 +7479,7 @@
         <v>0.3</v>
       </c>
       <c r="T88" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V88" s="19" t="s">
         <v>130</v>
@@ -7514,7 +7514,7 @@
       </c>
       <c r="O89" s="36">
         <f>O82*T89</f>
-        <v>2.4275000000000001E-2</v>
+        <v>4.8550000000000003E-2</v>
       </c>
       <c r="P89" s="16">
         <v>5</v>
@@ -7526,7 +7526,7 @@
         <v>0.3</v>
       </c>
       <c r="T89" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V89" s="19" t="s">
         <v>130</v>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="O98" s="35">
         <f>O92*T98</f>
-        <v>8.1000000000000006E-4</v>
+        <v>1.6200000000000001E-3</v>
       </c>
       <c r="P98" s="19">
         <v>5</v>
@@ -8040,7 +8040,7 @@
         <v>0.3</v>
       </c>
       <c r="T98" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V98" s="19" t="s">
         <v>130</v>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="O99" s="35">
         <f t="shared" si="68"/>
-        <v>3.5699999999999998E-3</v>
+        <v>7.1399999999999996E-3</v>
       </c>
       <c r="P99" s="19">
         <v>5</v>
@@ -8087,7 +8087,7 @@
         <v>0.3</v>
       </c>
       <c r="T99" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V99" s="19" t="s">
         <v>130</v>
@@ -8122,7 +8122,7 @@
       </c>
       <c r="O100" s="36">
         <f t="shared" si="68"/>
-        <v>0.43785499999999999</v>
+        <v>0.87570999999999999</v>
       </c>
       <c r="P100" s="16">
         <v>5</v>
@@ -8134,7 +8134,7 @@
         <v>0.3</v>
       </c>
       <c r="T100" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V100" s="19" t="s">
         <v>130</v>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="O107" s="35">
         <f>O102*T107</f>
-        <v>3.4249999999999997E-3</v>
+        <v>6.8499999999999993E-3</v>
       </c>
       <c r="P107" s="19">
         <v>5</v>
@@ -8563,7 +8563,7 @@
         <v>0.3</v>
       </c>
       <c r="T107" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V107" s="19"/>
       <c r="W107" s="19"/>
@@ -8626,7 +8626,7 @@
       </c>
       <c r="O108" s="35">
         <f t="shared" si="80"/>
-        <v>3.4619999999999998E-2</v>
+        <v>6.9239999999999996E-2</v>
       </c>
       <c r="P108" s="19">
         <v>5</v>
@@ -8638,7 +8638,7 @@
         <v>0.3</v>
       </c>
       <c r="T108" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V108" t="s">
         <v>130</v>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="O109" s="36">
         <f t="shared" si="80"/>
-        <v>0.12943499999999999</v>
+        <v>0.25886999999999999</v>
       </c>
       <c r="P109" s="16">
         <v>5</v>
@@ -8685,7 +8685,7 @@
         <v>0.3</v>
       </c>
       <c r="T109" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V109" t="s">
         <v>130</v>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="O116" s="35">
         <f>O111*T116</f>
-        <v>2.2099999999999997E-3</v>
+        <v>4.4199999999999995E-3</v>
       </c>
       <c r="P116" s="19">
         <v>5</v>
@@ -9114,7 +9114,7 @@
         <v>0.3</v>
       </c>
       <c r="T116" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V116" s="19"/>
       <c r="W116" s="19"/>
@@ -9177,7 +9177,7 @@
       </c>
       <c r="O117" s="35">
         <f t="shared" si="92"/>
-        <v>4.8649999999999995E-3</v>
+        <v>9.7299999999999991E-3</v>
       </c>
       <c r="P117" s="19">
         <v>5</v>
@@ -9189,7 +9189,7 @@
         <v>0.3</v>
       </c>
       <c r="T117" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V117" t="s">
         <v>130</v>
@@ -9224,7 +9224,7 @@
       </c>
       <c r="O118" s="36">
         <f t="shared" si="92"/>
-        <v>9.018000000000001E-2</v>
+        <v>0.18036000000000002</v>
       </c>
       <c r="P118" s="16">
         <v>5</v>
@@ -9236,7 +9236,7 @@
         <v>0.3</v>
       </c>
       <c r="T118" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V118" t="s">
         <v>130</v>
@@ -9653,7 +9653,7 @@
       </c>
       <c r="O125" s="35">
         <f>O120*T125</f>
-        <v>6.6449999999999999E-3</v>
+        <v>1.329E-2</v>
       </c>
       <c r="P125" s="19">
         <v>5</v>
@@ -9665,7 +9665,7 @@
         <v>0.3</v>
       </c>
       <c r="T125" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V125" s="19"/>
       <c r="W125" s="19"/>
@@ -9728,7 +9728,7 @@
       </c>
       <c r="O126" s="35">
         <f t="shared" si="104"/>
-        <v>5.5189999999999996E-2</v>
+        <v>0.11037999999999999</v>
       </c>
       <c r="P126" s="19">
         <v>5</v>
@@ -9740,7 +9740,7 @@
         <v>0.3</v>
       </c>
       <c r="T126" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V126" t="s">
         <v>130</v>
@@ -9787,7 +9787,7 @@
         <v>0.3</v>
       </c>
       <c r="T127" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V127" t="s">
         <v>130</v>
@@ -10261,7 +10261,7 @@
       </c>
       <c r="O135" s="35">
         <f>O129*T135</f>
-        <v>3.7599999999999999E-3</v>
+        <v>7.5199999999999998E-3</v>
       </c>
       <c r="P135" s="19">
         <v>5</v>
@@ -10273,7 +10273,7 @@
         <v>0.3</v>
       </c>
       <c r="T135" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V135" s="19" t="s">
         <v>130</v>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="O136" s="35">
         <f t="shared" si="116"/>
-        <v>1.5594999999999999E-2</v>
+        <v>3.1189999999999999E-2</v>
       </c>
       <c r="P136" s="19">
         <v>5</v>
@@ -10324,7 +10324,7 @@
         <v>0.3</v>
       </c>
       <c r="T136" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V136" t="s">
         <v>130</v>
@@ -10359,7 +10359,7 @@
       </c>
       <c r="O137" s="36">
         <f t="shared" si="116"/>
-        <v>0.14768000000000001</v>
+        <v>0.29536000000000001</v>
       </c>
       <c r="P137" s="16">
         <v>5</v>
@@ -10371,7 +10371,7 @@
         <v>0.3</v>
       </c>
       <c r="T137" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V137" t="s">
         <v>130</v>
@@ -10788,7 +10788,7 @@
       </c>
       <c r="O144" s="35">
         <f>O139*T144</f>
-        <v>3.7599999999999999E-3</v>
+        <v>7.5199999999999998E-3</v>
       </c>
       <c r="P144" s="19">
         <v>5</v>
@@ -10800,7 +10800,7 @@
         <v>0.3</v>
       </c>
       <c r="T144" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V144" s="19"/>
       <c r="W144" s="19"/>
@@ -10865,7 +10865,7 @@
       </c>
       <c r="O145" s="35">
         <f t="shared" si="128"/>
-        <v>0.26459499999999997</v>
+        <v>0.52918999999999994</v>
       </c>
       <c r="P145" s="19">
         <v>5</v>
@@ -10877,7 +10877,7 @@
         <v>0.3</v>
       </c>
       <c r="T145" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="7:20" x14ac:dyDescent="0.25">
@@ -10909,7 +10909,7 @@
       </c>
       <c r="O146" s="36">
         <f t="shared" si="128"/>
-        <v>0.10112</v>
+        <v>0.20224</v>
       </c>
       <c r="P146" s="16">
         <v>5</v>
@@ -10921,7 +10921,7 @@
         <v>0.3</v>
       </c>
       <c r="T146" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include existing biomass in calculating max coal/coke/h2/biomass consumption share in cement production
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_IND_Mitigations.xlsx
+++ b/SuppXLS/Scen_IND_Mitigations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\2-NewVeda\TIMES-Ireland-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0521E49-B58F-4E37-B58A-A11985A6945D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AE468D-8F1D-464E-AA78-CFDA881D3AA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="148">
   <si>
     <t>Development</t>
   </si>
@@ -671,9 +671,6 @@
     <t>NRGI</t>
   </si>
   <si>
-    <t>Basae year data</t>
-  </si>
-  <si>
     <t>User Input Data</t>
   </si>
   <si>
@@ -711,6 +708,12 @@
   </si>
   <si>
     <t>I-DMD-ONM-*</t>
+  </si>
+  <si>
+    <t>Base year data</t>
+  </si>
+  <si>
+    <t>*2018</t>
   </si>
 </sst>
 </file>
@@ -2245,8 +2248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V90" sqref="V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,12 +2292,12 @@
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.25">
       <c r="M3" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="R3" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
@@ -2313,14 +2316,14 @@
         <v>~TFM_INS-TS:IE,National</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V4" s="9"/>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="AA4" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AB4" s="9"/>
       <c r="AC4" s="9"/>
@@ -2394,13 +2397,13 @@
         <v>64</v>
       </c>
       <c r="Z5" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" s="11">
-        <v>2018</v>
+      <c r="AB5" s="11" t="s">
+        <v>147</v>
       </c>
       <c r="AC5" s="11">
         <v>2020</v>
@@ -2412,7 +2415,7 @@
         <v>2050</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>127</v>
@@ -2436,7 +2439,7 @@
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="19" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
@@ -2518,10 +2521,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y7" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z7" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA7" s="28" t="s">
         <v>131</v>
@@ -2592,10 +2595,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y8" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z8" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA8" s="28" t="s">
         <v>131</v>
@@ -2682,7 +2685,7 @@
         <v>IND*</v>
       </c>
       <c r="Z9" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA9" s="28" t="str">
         <f>$AA$7</f>
@@ -2757,10 +2760,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y10" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z10" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA10" s="28" t="str">
         <f>$AA$7</f>
@@ -2838,7 +2841,7 @@
         <v>IND*</v>
       </c>
       <c r="Z11" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA11" s="28" t="str">
         <f>$AA$7</f>
@@ -2923,10 +2926,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y12" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z12" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA12" s="28" t="str">
         <f>$AA$7</f>
@@ -3167,10 +3170,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y16" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z16" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA16" s="42" t="str">
         <f>$AA$20</f>
@@ -3241,10 +3244,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y17" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z17" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA17" s="42" t="str">
         <f>$AA$20</f>
@@ -3330,7 +3333,7 @@
         <v>IND*</v>
       </c>
       <c r="Z18" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA18" s="42" t="str">
         <f>$AA$20</f>
@@ -3401,10 +3404,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y19" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z19" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA19" s="42" t="str">
         <f>$AA$20</f>
@@ -3477,7 +3480,7 @@
         <v>IND*</v>
       </c>
       <c r="Z20" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA20" s="28" t="s">
         <v>131</v>
@@ -3557,10 +3560,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y21" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z21" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA21" s="28" t="s">
         <v>131</v>
@@ -3986,10 +3989,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y29" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z29" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA29" s="42" t="str">
         <f>$AA$20</f>
@@ -4060,10 +4063,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y30" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z30" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA30" s="42" t="str">
         <f>$AA$20</f>
@@ -4149,7 +4152,7 @@
         <v>IND*</v>
       </c>
       <c r="Z31" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA31" s="42" t="str">
         <f>$AA$20</f>
@@ -4223,10 +4226,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y32" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z32" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA32" s="42" t="str">
         <f>$AA$20</f>
@@ -4257,7 +4260,7 @@
         <v>76</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>109</v>
@@ -4303,7 +4306,7 @@
         <v>IND*</v>
       </c>
       <c r="Z33" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA33" s="28" t="s">
         <v>131</v>
@@ -4339,7 +4342,7 @@
         <v>76</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>110</v>
@@ -4392,10 +4395,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y34" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z34" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA34" s="28" t="s">
         <v>131</v>
@@ -4425,7 +4428,7 @@
         <v>76</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" s="31" t="s">
         <v>80</v>
@@ -4484,10 +4487,10 @@
         <v>76</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G36" s="38" t="s">
         <v>130</v>
@@ -4632,10 +4635,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y38" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z38" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA38" s="42" t="str">
         <f>$AA$20</f>
@@ -4706,10 +4709,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y39" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z39" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA39" s="42" t="str">
         <f>$AA$20</f>
@@ -4795,7 +4798,7 @@
         <v>IND*</v>
       </c>
       <c r="Z40" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA40" s="42" t="str">
         <f>$AA$20</f>
@@ -4869,10 +4872,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y41" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z41" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA41" s="42" t="str">
         <f>$AA$20</f>
@@ -4949,7 +4952,7 @@
         <v>IND*</v>
       </c>
       <c r="Z42" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA42" s="28" t="s">
         <v>131</v>
@@ -5020,10 +5023,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y43" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z43" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA43" s="28" t="s">
         <v>131</v>
@@ -5319,10 +5322,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y48" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z48" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA48" s="42" t="str">
         <f>$AA$20</f>
@@ -5387,10 +5390,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y49" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z49" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA49" s="42" t="str">
         <f>$AA$20</f>
@@ -5476,7 +5479,7 @@
         <v>IND*</v>
       </c>
       <c r="Z50" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA50" s="42" t="str">
         <f>$AA$20</f>
@@ -5556,10 +5559,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y51" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z51" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA51" s="42" t="str">
         <f>$AA$20</f>
@@ -5636,7 +5639,7 @@
         <v>IND*</v>
       </c>
       <c r="Z52" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA52" s="28" t="s">
         <v>131</v>
@@ -5718,10 +5721,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y53" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z53" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA53" s="28" t="s">
         <v>131</v>
@@ -5958,10 +5961,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y57" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z57" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA57" s="42" t="str">
         <f>$AA$20</f>
@@ -6032,10 +6035,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y58" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z58" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA58" s="42" t="str">
         <f>$AA$20</f>
@@ -6112,7 +6115,7 @@
         <v>IND*</v>
       </c>
       <c r="Z59" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA59" s="42" t="str">
         <f>$AA$20</f>
@@ -6194,10 +6197,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y60" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z60" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA60" s="42" t="str">
         <f>$AA$20</f>
@@ -6268,7 +6271,7 @@
         <v>IND*</v>
       </c>
       <c r="Z61" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA61" s="28" t="s">
         <v>131</v>
@@ -6340,10 +6343,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y62" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z62" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA62" s="28" t="s">
         <v>131</v>
@@ -6614,10 +6617,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y68" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z68" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA68" s="42" t="str">
         <f>$AA$20</f>
@@ -6676,10 +6679,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y69" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z69" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA69" s="42" t="str">
         <f>$AA$20</f>
@@ -6753,7 +6756,7 @@
         <v>IND*</v>
       </c>
       <c r="Z70" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA70" s="42" t="str">
         <f>$AA$20</f>
@@ -6821,10 +6824,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y71" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z71" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA71" s="42" t="str">
         <f>$AA$20</f>
@@ -6889,7 +6892,7 @@
         <v>IND*</v>
       </c>
       <c r="Z72" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA72" s="28" t="s">
         <v>131</v>
@@ -6967,10 +6970,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y73" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z73" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA73" s="28" t="s">
         <v>131</v>
@@ -7129,7 +7132,7 @@
         <v>132</v>
       </c>
       <c r="J77" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K77" s="37" t="s">
         <v>65</v>
@@ -7165,10 +7168,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y77" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z77" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA77" s="42" t="str">
         <f>$AA$20</f>
@@ -7208,7 +7211,7 @@
         <v>132</v>
       </c>
       <c r="J78" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K78" s="37" t="s">
         <v>67</v>
@@ -7236,10 +7239,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y78" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z78" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA78" s="42" t="str">
         <f>$AA$20</f>
@@ -7273,7 +7276,7 @@
         <v>132</v>
       </c>
       <c r="J79" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K79" s="37" t="s">
         <v>69</v>
@@ -7304,7 +7307,7 @@
         <v>IND*</v>
       </c>
       <c r="Z79" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA79" s="42" t="str">
         <f>$AA$20</f>
@@ -7344,7 +7347,7 @@
         <v>132</v>
       </c>
       <c r="J80" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K80" s="37" t="s">
         <v>70</v>
@@ -7372,10 +7375,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y80" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z80" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA80" s="42" t="str">
         <f>$AA$20</f>
@@ -7409,7 +7412,7 @@
         <v>132</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K81" s="37" t="s">
         <v>71</v>
@@ -7449,7 +7452,7 @@
         <v>IND*</v>
       </c>
       <c r="Z81" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA81" s="28" t="s">
         <v>131</v>
@@ -7488,7 +7491,7 @@
         <v>132</v>
       </c>
       <c r="J82" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K82" s="37" t="s">
         <v>72</v>
@@ -7518,10 +7521,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y82" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z82" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA82" s="28" t="s">
         <v>131</v>
@@ -7555,7 +7558,7 @@
         <v>132</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K83" s="37" t="s">
         <v>78</v>
@@ -7586,26 +7589,26 @@
         <v>IND*</v>
       </c>
       <c r="Z83" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA83" s="28" t="s">
         <v>131</v>
       </c>
       <c r="AB83" s="29">
         <f>1+AB84</f>
-        <v>0.48587000000000002</v>
+        <v>0.48062000000000005</v>
       </c>
       <c r="AC83" s="29">
         <f t="shared" si="56"/>
-        <v>0.48587000000000002</v>
+        <v>0.48062000000000005</v>
       </c>
       <c r="AD83" s="29">
         <f t="shared" si="57"/>
-        <v>0.48587000000000002</v>
+        <v>0.48062000000000005</v>
       </c>
       <c r="AE83" s="29">
         <f t="shared" si="58"/>
-        <v>0.48587000000000002</v>
+        <v>0.48062000000000005</v>
       </c>
       <c r="AF83" s="30">
         <v>0</v>
@@ -7625,7 +7628,7 @@
         <v>132</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K84" s="37" t="s">
         <v>81</v>
@@ -7667,29 +7670,29 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y84" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Z84" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA84" s="28" t="s">
         <v>131</v>
       </c>
       <c r="AB84" s="43">
-        <f>-L77-L81</f>
-        <v>-0.51412999999999998</v>
+        <f>-L77-L81-$L$84</f>
+        <v>-0.51937999999999995</v>
       </c>
       <c r="AC84" s="43">
-        <f t="shared" ref="AC84:AE84" si="60">-M77-M81</f>
-        <v>-0.51412999999999998</v>
+        <f t="shared" ref="AC84:AE84" si="60">-M77-M81-$L$84</f>
+        <v>-0.51937999999999995</v>
       </c>
       <c r="AD84" s="43">
         <f t="shared" si="60"/>
-        <v>-0.51412999999999998</v>
+        <v>-0.51937999999999995</v>
       </c>
       <c r="AE84" s="43">
         <f t="shared" si="60"/>
-        <v>-0.51412999999999998</v>
+        <v>-0.51937999999999995</v>
       </c>
       <c r="AF84" s="37"/>
     </row>
@@ -7704,7 +7707,7 @@
         <v>132</v>
       </c>
       <c r="J85" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K85" s="37" t="s">
         <v>87</v>
@@ -7736,7 +7739,7 @@
         <v>132</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K86" s="37" t="s">
         <v>88</v>
@@ -7768,7 +7771,7 @@
         <v>132</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K87" s="37" t="s">
         <v>109</v>
@@ -7815,7 +7818,7 @@
         <v>132</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K88" s="37" t="s">
         <v>110</v>
@@ -7862,7 +7865,7 @@
         <v>132</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K89" s="37" t="s">
         <v>80</v>
@@ -7908,11 +7911,11 @@
       <c r="I90" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="J90" s="25" t="s">
-        <v>146</v>
+      <c r="J90" s="33" t="s">
+        <v>145</v>
       </c>
       <c r="K90" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L90" s="39">
         <v>0</v>
@@ -8018,10 +8021,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y92" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z92" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA92" s="42" t="str">
         <f>$AA$20</f>
@@ -8089,10 +8092,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y93" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z93" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA93" s="42" t="str">
         <f>$AA$20</f>
@@ -8157,7 +8160,7 @@
         <v>IND*</v>
       </c>
       <c r="Z94" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA94" s="42" t="str">
         <f>$AA$20</f>
@@ -8216,10 +8219,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y95" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z95" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA95" s="42" t="str">
         <f>$AA$20</f>
@@ -8293,7 +8296,7 @@
         <v>IND*</v>
       </c>
       <c r="Z96" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA96" s="28" t="s">
         <v>131</v>
@@ -8370,10 +8373,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y97" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z97" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA97" s="28" t="s">
         <v>131</v>
@@ -8635,10 +8638,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y103" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z103" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA103" s="42" t="str">
         <f>$AA$20</f>
@@ -8697,10 +8700,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y104" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z104" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA104" s="42" t="str">
         <f>$AA$20</f>
@@ -8774,7 +8777,7 @@
         <v>IND*</v>
       </c>
       <c r="Z105" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA105" s="42" t="str">
         <f>$AA$20</f>
@@ -8851,10 +8854,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y106" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z106" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA106" s="42" t="str">
         <f>$AA$20</f>
@@ -8928,7 +8931,7 @@
         <v>IND*</v>
       </c>
       <c r="Z107" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA107" s="28" t="s">
         <v>131</v>
@@ -9006,10 +9009,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y108" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z108" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA108" s="28" t="s">
         <v>131</v>
@@ -9186,10 +9189,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y112" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z112" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA112" s="42" t="str">
         <f>$AA$20</f>
@@ -9248,10 +9251,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y113" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z113" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA113" s="42" t="str">
         <f>$AA$20</f>
@@ -9325,7 +9328,7 @@
         <v>IND*</v>
       </c>
       <c r="Z114" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA114" s="42" t="str">
         <f>$AA$20</f>
@@ -9402,10 +9405,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y115" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z115" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA115" s="42" t="str">
         <f>$AA$20</f>
@@ -9479,7 +9482,7 @@
         <v>IND*</v>
       </c>
       <c r="Z116" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA116" s="28" t="s">
         <v>131</v>
@@ -9557,10 +9560,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y117" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z117" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA117" s="28" t="s">
         <v>131</v>
@@ -9737,10 +9740,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y121" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z121" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA121" s="42" t="str">
         <f>$AA$20</f>
@@ -9799,10 +9802,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y122" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z122" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA122" s="42" t="str">
         <f>$AA$20</f>
@@ -9876,7 +9879,7 @@
         <v>IND*</v>
       </c>
       <c r="Z123" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA123" s="42" t="str">
         <f>$AA$20</f>
@@ -9953,10 +9956,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y124" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z124" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA124" s="42" t="str">
         <f>$AA$20</f>
@@ -10030,7 +10033,7 @@
         <v>IND*</v>
       </c>
       <c r="Z125" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA125" s="28" t="s">
         <v>131</v>
@@ -10108,10 +10111,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y126" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z126" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA126" s="28" t="s">
         <v>131</v>
@@ -10288,10 +10291,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y130" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z130" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA130" s="42" t="str">
         <f>$AA$20</f>
@@ -10350,10 +10353,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y131" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z131" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA131" s="42" t="str">
         <f>$AA$20</f>
@@ -10418,7 +10421,7 @@
         <v>IND*</v>
       </c>
       <c r="Z132" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA132" s="42" t="str">
         <f>$AA$20</f>
@@ -10486,10 +10489,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y133" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z133" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA133" s="42" t="str">
         <f>$AA$20</f>
@@ -10572,7 +10575,7 @@
         <v>IND*</v>
       </c>
       <c r="Z134" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA134" s="28" t="s">
         <v>131</v>
@@ -10641,10 +10644,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y135" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z135" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA135" s="28" t="s">
         <v>131</v>
@@ -10872,10 +10875,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y140" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z140" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA140" s="42" t="str">
         <f>$AA$20</f>
@@ -10934,10 +10937,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y141" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z141" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA141" s="42" t="str">
         <f>$AA$20</f>
@@ -11011,7 +11014,7 @@
         <v>IND*</v>
       </c>
       <c r="Z142" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA142" s="42" t="str">
         <f>$AA$20</f>
@@ -11088,10 +11091,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y143" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z143" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA143" s="42" t="str">
         <f>$AA$20</f>
@@ -11165,7 +11168,7 @@
         <v>IND*</v>
       </c>
       <c r="Z144" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA144" s="28" t="s">
         <v>131</v>
@@ -11243,10 +11246,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y145" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z145" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA145" s="28" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Allow to substitute diesel with biodiesel in food and beverages (IND)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_IND_Mitigations.xlsx
+++ b/SuppXLS/Scen_IND_Mitigations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AE468D-8F1D-464E-AA78-CFDA881D3AA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCFD275-30E4-432A-9936-C16E77C22F22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="148">
   <si>
     <t>Development</t>
   </si>
@@ -968,7 +968,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1126,6 +1126,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2248,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V90" sqref="V90"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,16 +2790,16 @@
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="31" t="s">
         <v>109</v>
       </c>
       <c r="F11" s="21"/>
@@ -2871,12 +2874,18 @@
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="G12" s="16" t="s">
         <v>130</v>
       </c>
@@ -2955,18 +2964,12 @@
       <c r="AG12" s="37"/>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B13" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="G13" s="16" t="s">
         <v>130</v>
       </c>
@@ -3023,8 +3026,8 @@
       <c r="D14" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>110</v>
+      <c r="E14" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G14" s="38" t="s">
         <v>130</v>
@@ -3084,17 +3087,17 @@
       <c r="AG14" s="38"/>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>80</v>
+      <c r="E15" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>96</v>
@@ -3127,12 +3130,18 @@
       <c r="AG15" s="23"/>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G16" s="16" t="s">
         <v>130</v>
       </c>
@@ -3203,18 +3212,12 @@
       </c>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B17" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="G17" s="16" t="s">
         <v>130</v>
       </c>
@@ -3280,8 +3283,8 @@
       <c r="D18" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="31" t="s">
-        <v>110</v>
+      <c r="E18" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>130</v>
@@ -3363,17 +3366,17 @@
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="34" t="s">
-        <v>80</v>
+      <c r="E19" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>130</v>
@@ -3433,12 +3436,18 @@
       <c r="AG19" s="37"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="B20" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G20" s="16" t="s">
         <v>130</v>
       </c>
@@ -3509,18 +3518,12 @@
       </c>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
       <c r="G21" s="16" t="s">
         <v>130</v>
       </c>
@@ -3595,8 +3598,8 @@
       <c r="D22" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="31" t="s">
-        <v>110</v>
+      <c r="E22" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>130</v>
@@ -3636,17 +3639,17 @@
       </c>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>80</v>
+      <c r="E23" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>130</v>
@@ -3677,12 +3680,18 @@
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G24" s="16" t="s">
         <v>130</v>
       </c>
@@ -3730,18 +3739,12 @@
       </c>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B25" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
       <c r="G25" s="37" t="s">
         <v>130</v>
       </c>
@@ -3784,8 +3787,8 @@
       <c r="D26" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>110</v>
+      <c r="E26" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G26" s="37" t="s">
         <v>130</v>
@@ -3834,17 +3837,17 @@
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="34" t="s">
-        <v>80</v>
+      <c r="E27" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G27" s="38" t="s">
         <v>130</v>
@@ -3894,12 +3897,18 @@
       <c r="Z27" s="38"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="B28" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G28" s="19" t="s">
         <v>97</v>
       </c>
@@ -3931,18 +3940,12 @@
       <c r="AG28" s="49"/>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B29" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
       <c r="G29" s="37" t="s">
         <v>130</v>
       </c>
@@ -4031,8 +4034,8 @@
       <c r="D30" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="31" t="s">
-        <v>110</v>
+      <c r="E30" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>130</v>
@@ -4090,17 +4093,17 @@
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="34" t="s">
-        <v>80</v>
+      <c r="E31" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>130</v>
@@ -4182,12 +4185,18 @@
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="B32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G32" s="37" t="s">
         <v>130</v>
       </c>
@@ -4253,18 +4262,12 @@
       </c>
     </row>
     <row r="33" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B33" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
       <c r="G33" s="37" t="s">
         <v>130</v>
       </c>
@@ -4344,8 +4347,8 @@
       <c r="D34" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="31" t="s">
-        <v>110</v>
+      <c r="E34" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G34" s="37" t="s">
         <v>130</v>
@@ -4427,11 +4430,11 @@
       <c r="C35" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="25" t="s">
         <v>145</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>130</v>
@@ -4480,17 +4483,17 @@
       </c>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="34" t="s">
-        <v>143</v>
+      <c r="E36" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="G36" s="38" t="s">
         <v>130</v>
@@ -4540,12 +4543,18 @@
       <c r="Z36" s="38"/>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="B37" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>143</v>
+      </c>
       <c r="G37" s="19" t="s">
         <v>98</v>
       </c>
@@ -4577,18 +4586,12 @@
       <c r="AG37" s="49"/>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B38" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
       <c r="G38" s="37" t="s">
         <v>130</v>
       </c>
@@ -4677,8 +4680,8 @@
       <c r="D39" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="31" t="s">
-        <v>110</v>
+      <c r="E39" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>130</v>
@@ -4736,17 +4739,17 @@
       </c>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="34" t="s">
-        <v>80</v>
+      <c r="E40" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G40" s="37" t="s">
         <v>130</v>
@@ -4828,12 +4831,18 @@
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+      <c r="B41" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G41" s="37" t="s">
         <v>130</v>
       </c>
@@ -4899,18 +4908,12 @@
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B42" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
       <c r="G42" s="37" t="s">
         <v>130</v>
       </c>
@@ -4990,8 +4993,8 @@
       <c r="D43" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="31" t="s">
-        <v>110</v>
+      <c r="E43" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G43" s="37" t="s">
         <v>130</v>
@@ -5049,17 +5052,17 @@
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="34" t="s">
-        <v>80</v>
+      <c r="E44" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G44" s="37" t="s">
         <v>130</v>
@@ -5108,12 +5111,18 @@
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B45" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="B45" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G45" s="37" t="s">
         <v>130</v>
       </c>
@@ -5161,18 +5170,12 @@
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B46" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
       <c r="G46" s="38" t="s">
         <v>130</v>
       </c>
@@ -5230,8 +5233,8 @@
       <c r="D47" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="31" t="s">
-        <v>110</v>
+      <c r="E47" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G47" s="19" t="s">
         <v>99</v>
@@ -5264,17 +5267,17 @@
       <c r="AG47" s="49"/>
     </row>
     <row r="48" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E48" s="34" t="s">
-        <v>80</v>
+      <c r="E48" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G48" s="37" t="s">
         <v>130</v>
@@ -5355,12 +5358,18 @@
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B49" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
+      <c r="B49" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G49" s="37" t="s">
         <v>130</v>
       </c>
@@ -5417,18 +5426,12 @@
       </c>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B50" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
       <c r="G50" s="37" t="s">
         <v>130</v>
       </c>
@@ -5518,8 +5521,8 @@
       <c r="D51" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E51" s="31" t="s">
-        <v>110</v>
+      <c r="E51" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G51" s="37" t="s">
         <v>130</v>
@@ -5586,17 +5589,17 @@
       </c>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="33" t="s">
+      <c r="D52" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="34" t="s">
-        <v>80</v>
+      <c r="E52" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G52" s="37" t="s">
         <v>130</v>
@@ -5668,12 +5671,18 @@
       </c>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B53" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
+      <c r="B53" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G53" s="37" t="s">
         <v>130</v>
       </c>
@@ -5747,18 +5756,12 @@
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B54" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
       <c r="G54" s="37" t="s">
         <v>130</v>
       </c>
@@ -5812,11 +5815,11 @@
       <c r="C55" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E55" s="31" t="s">
-        <v>110</v>
+      <c r="E55" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G55" s="38" t="s">
         <v>130</v>
@@ -5866,17 +5869,17 @@
       <c r="Z55" s="38"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="34" t="s">
-        <v>80</v>
+      <c r="E56" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="G56" s="19" t="s">
         <v>100</v>
@@ -5909,12 +5912,18 @@
       <c r="AG56" s="49"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="B57" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="G57" s="37" t="s">
         <v>130</v>
       </c>
@@ -5994,18 +6003,12 @@
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B58" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="B58" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
       <c r="G58" s="37" t="s">
         <v>130</v>
       </c>
@@ -6071,8 +6074,8 @@
       <c r="D59" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E59" s="31" t="s">
-        <v>110</v>
+      <c r="E59" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="G59" s="37" t="s">
         <v>130</v>
@@ -6156,7 +6159,7 @@
         <v>94</v>
       </c>
       <c r="E60" s="31" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F60" s="37"/>
       <c r="G60" s="37" t="s">
@@ -6225,10 +6228,18 @@
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="31"/>
+      <c r="B61" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>80</v>
+      </c>
       <c r="F61" s="37"/>
       <c r="G61" s="37" t="s">
         <v>130</v>
@@ -6369,6 +6380,10 @@
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="31"/>
       <c r="G63" s="37" t="s">
         <v>130</v>
       </c>

</xml_diff>